<commit_message>
Adding "informal label" as annotation property
</commit_message>
<xml_diff>
--- a/UpperLevel/GMHO_Upper_Rels.xlsx
+++ b/UpperLevel/GMHO_Upper_Rels.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,11 +479,6 @@
           <t>LSR no</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
           <t>AnnotationProperty</t>
@@ -506,14 +501,11 @@
           <t>has occurrent part [BFO:0000117]</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>Inverse of occurrent_part_of which is defined as: b occurrent_part_of c =Def. b is a part of c and b and c are occurrents.</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
           <t>ObjectProperty</t>
@@ -521,30 +513,45 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>BFO:0000055</t>
-        </is>
-      </c>
+      <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr">
         <is>
-          <t>realises</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>realizes [BFO:0000055]</t>
-        </is>
-      </c>
+          <t>informal label</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>To say that b realizes c at t is to assert that there is some material entity d and b is a process which has participant d at t and c is a disposition or role of which d is bearer_of at tand the type instantiated by b is correlated with the type instantiated by c.</t>
-        </is>
-      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
+        <is>
+          <t>AnnotationProperty</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>BFO:0000055</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>realises</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>realizes [BFO:0000055]</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>To say that b realizes c at t is to assert that there is some material entity d and b is a process which has participant d at t and c is a disposition or role of which d is bearer_of at tand the type instantiated by b is correlated with the type instantiated by c.</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
         <is>
           <t>ObjectProperty</t>
         </is>

</xml_diff>